<commit_message>
mass_upload error handling in progress
</commit_message>
<xml_diff>
--- a/mass_upload.xlsx
+++ b/mass_upload.xlsx
@@ -34,7 +34,7 @@
     <t>Phone Number*</t>
   </si>
   <si>
-    <t>Gender*</t>
+    <t>Gender*(Bro/Sis)</t>
   </si>
   <si>
     <t>Email</t>
@@ -171,6 +171,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="15.14"/>
+    <col customWidth="1" min="5" max="5" width="16.14"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -224,9 +225,7 @@
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1">
-        <v>8.134031365E9</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
mass upload - error handling - handle_none, validate gender
</commit_message>
<xml_diff>
--- a/mass_upload.xlsx
+++ b/mass_upload.xlsx
@@ -225,7 +225,9 @@
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>8.134031365E9</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>